<commit_message>
Auflistung der erlaubten Gemeinden
</commit_message>
<xml_diff>
--- a/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Werth.xlsx
+++ b/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Werth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Desktop\Schule\5. Jahrgang\SWP\Ferienspass\Taetigkeitsprotokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEDF833-2E2C-4981-BA2A-A8E439834EAE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B555C8E0-9C25-49DB-9191-E18D25A9F269}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Erstellen der Email-Klasse</t>
+  </si>
+  <si>
+    <t>10.12.2019</t>
+  </si>
+  <si>
+    <t>Sprintplaning und Programierung</t>
   </si>
 </sst>
 </file>
@@ -294,6 +300,18 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -317,18 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,7 +735,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -742,12 +748,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="8"/>
@@ -784,35 +790,35 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="39" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:13" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -864,12 +870,12 @@
         <v>5.555555555555558E-2</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -918,14 +924,24 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="28"/>
+      <c r="A11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="25">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D11" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.21874999999999994</v>
       </c>
       <c r="G11" s="11"/>
     </row>
@@ -1244,109 +1260,109 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="22">
         <f>SUM(F7:F37)</f>
-        <v>0.4826388888888889</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
       <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
@@ -1369,6 +1385,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A46:F46"/>
     <mergeCell ref="A47:F47"/>
     <mergeCell ref="A48:F48"/>
@@ -1378,15 +1403,6 @@
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Admineinstellungen: Anmeldezeitraum und Rabatt
</commit_message>
<xml_diff>
--- a/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Werth.xlsx
+++ b/Taetigkeitsprotokolle/Taetigkeitsprotokoll_Werth.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Desktop\Schule\5. Jahrgang\SWP\Ferienspass\Taetigkeitsprotokolle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\HTL\5. Jahrgang\SWP\Ferienspass\Taetigkeitsprotokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5BC063-B430-4E0A-A8B6-5142D6B6B36D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="882" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="882"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -114,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="[$-407]ddd"/>
@@ -306,6 +305,18 @@
     <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -329,18 +340,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,23 +492,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -545,23 +527,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -737,34 +702,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="64.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -773,7 +738,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:13" s="4" customFormat="1" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="4" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -786,7 +751,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:13" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -795,42 +760,42 @@
       <c r="F4" s="18"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="39" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>43775</v>
       </c>
@@ -855,7 +820,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>15</v>
       </c>
@@ -876,14 +841,14 @@
         <v>5.555555555555558E-2</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>15</v>
       </c>
@@ -906,7 +871,7 @@
       <c r="G9" s="11"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>15</v>
       </c>
@@ -929,7 +894,7 @@
       <c r="G10" s="11"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
@@ -951,7 +916,7 @@
       </c>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>15</v>
       </c>
@@ -973,7 +938,7 @@
       </c>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="24"/>
       <c r="C13" s="25"/>
@@ -985,7 +950,7 @@
       </c>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
@@ -997,7 +962,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
@@ -1009,7 +974,7 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
@@ -1021,7 +986,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="27"/>
       <c r="C17" s="25"/>
@@ -1033,7 +998,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="24"/>
       <c r="C18" s="25"/>
@@ -1045,7 +1010,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
       <c r="B19" s="24"/>
       <c r="C19" s="25"/>
@@ -1057,7 +1022,7 @@
       </c>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="24"/>
       <c r="C20" s="25"/>
@@ -1069,7 +1034,7 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="27"/>
       <c r="C21" s="25"/>
@@ -1081,7 +1046,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
       <c r="B22" s="27"/>
       <c r="C22" s="25"/>
@@ -1093,7 +1058,7 @@
       </c>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="27"/>
       <c r="C23" s="25"/>
@@ -1105,7 +1070,7 @@
       </c>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="27"/>
       <c r="C24" s="25"/>
@@ -1117,7 +1082,7 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="B25" s="27"/>
       <c r="C25" s="25"/>
@@ -1129,7 +1094,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
       <c r="C26" s="25"/>
@@ -1141,7 +1106,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="25"/>
@@ -1153,7 +1118,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="27"/>
       <c r="B28" s="27"/>
       <c r="C28" s="25"/>
@@ -1165,7 +1130,7 @@
       </c>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="27"/>
       <c r="C29" s="25"/>
@@ -1177,7 +1142,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="27"/>
       <c r="C30" s="25"/>
@@ -1189,7 +1154,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="B31" s="27"/>
       <c r="C31" s="25"/>
@@ -1201,7 +1166,7 @@
       </c>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="27"/>
       <c r="C32" s="25"/>
@@ -1213,7 +1178,7 @@
       </c>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
       <c r="C33" s="25"/>
@@ -1225,7 +1190,7 @@
       </c>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="27"/>
       <c r="B34" s="27" t="s">
         <v>11</v>
@@ -1239,7 +1204,7 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="27"/>
       <c r="B35" s="27"/>
       <c r="C35" s="25"/>
@@ -1251,7 +1216,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="27"/>
       <c r="B36" s="27"/>
       <c r="C36" s="25"/>
@@ -1263,7 +1228,7 @@
       </c>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
       <c r="C37" s="25"/>
@@ -1275,113 +1240,113 @@
       </c>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="s">
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="22">
         <f>SUM(F7:F37)</f>
         <v>0.92013888888888884</v>
       </c>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
+    <row r="39" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="30" t="s">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
+    <row r="41" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="40"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+    <row r="43" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
+    <row r="45" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
+    <row r="47" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -1390,7 +1355,7 @@
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
     </row>
-    <row r="50" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -1401,6 +1366,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A46:F46"/>
     <mergeCell ref="A47:F47"/>
     <mergeCell ref="A48:F48"/>
@@ -1410,15 +1384,6 @@
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>